<commit_message>
Tudo funcionando, mas tá Lento!!
</commit_message>
<xml_diff>
--- a/envio_rendimentos/arquivos_gerados/EMPRESAS_NOMECURTO_CNPJ.xlsx
+++ b/envio_rendimentos/arquivos_gerados/EMPRESAS_NOMECURTO_CNPJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PGC\envio_rendimentos\arquivos_gerados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{706A2519-FBDD-4760-A83B-54197487C45C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1585ACD-07A1-4B54-9150-16254FDB8A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9C6E5FCC-DFCE-4D73-A9A7-EAE5958E03F6}"/>
   </bookViews>
@@ -36,95 +36,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>Nome completo</t>
-  </si>
-  <si>
-    <t>Nome curto</t>
-  </si>
-  <si>
-    <t>Cnpj</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+  <si>
+    <t>34.028.040/0003-25</t>
+  </si>
+  <si>
+    <t>48.896.217/0024-44</t>
+  </si>
+  <si>
+    <t>17.991.041/0001-90</t>
+  </si>
+  <si>
+    <t>23.585.934/0003-08</t>
+  </si>
+  <si>
+    <t>08.705.893/0001-82</t>
+  </si>
+  <si>
+    <t>30.182.622/0004-91</t>
+  </si>
+  <si>
+    <t>40.024.035/0001-85</t>
+  </si>
+  <si>
+    <t>30.145.972/0002-16</t>
+  </si>
+  <si>
+    <t>nome_curto</t>
+  </si>
+  <si>
+    <t>cnpj</t>
+  </si>
+  <si>
+    <t>nome_completo</t>
   </si>
   <si>
     <t>119 - RISERVA DOS VINHEDOS INCORPORADORA SPE LTDA</t>
   </si>
   <si>
-    <t>RISERVA</t>
-  </si>
-  <si>
-    <t>34.028.040/0003-25</t>
-  </si>
-  <si>
     <t>24 - LGM PARTICIPACOES LTDA | FILIAL PEDRAS ALTAS</t>
   </si>
   <si>
-    <t>JPZ/LGM</t>
-  </si>
-  <si>
-    <t>48.896.217/0024-44</t>
-  </si>
-  <si>
     <t>3 - GVP PARTICIPAÇÕES E INVESTIMENTOS LTDA</t>
   </si>
   <si>
-    <t>GVP</t>
-  </si>
-  <si>
-    <t>17.991.041/0001-90</t>
-  </si>
-  <si>
     <t>40 - GOLDEN LAGHETTO EMPREENDIMENTOS IMOBILIARIOS SPE LTDA</t>
   </si>
   <si>
-    <t>GOLDEN</t>
-  </si>
-  <si>
-    <t>23.585.934/0003-08</t>
-  </si>
-  <si>
     <t>68 - ATHIVABRASIL EMPREENDIMENTOS IMOBILIÁRIOS LTDA</t>
   </si>
   <si>
-    <t>ATHIVABRASIL</t>
-  </si>
-  <si>
-    <t>08.705.893/0001-82</t>
-  </si>
-  <si>
     <t>74 - ASA DELTA EMPREENDIMENTOS IMOBILIARIOS LTDA</t>
   </si>
   <si>
-    <t>ASA DELTA</t>
-  </si>
-  <si>
-    <t>30.182.622/0004-91</t>
-  </si>
-  <si>
     <t>2 - ALTOS DA BORGES EMPREENDIMENTOS IMOBILIARIOS LTDA</t>
   </si>
   <si>
-    <t>ALTOS DA BORGES</t>
-  </si>
-  <si>
-    <t>40.024.035/0001-85</t>
-  </si>
-  <si>
     <t>72 - CANELA EMPREENDIMENTOS IMOBILIARIOS LTDA</t>
-  </si>
-  <si>
-    <t>CANELA</t>
-  </si>
-  <si>
-    <t>30.145.972/0002-16</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -152,8 +136,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,7 +476,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A9" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -503,101 +488,101 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>